<commit_message>
new data for ML
</commit_message>
<xml_diff>
--- a/course_project/data/df_pv_data_germany.xlsx
+++ b/course_project/data/df_pv_data_germany.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi Eckmann\Desktop\ETH Studium\MASTERSTUDIUM\2. Semester\Big Data for Public Policy\big_data_policy_2020\course_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390D798-53A3-4E84-811A-3270020FB925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37760D3B-C081-4AAF-8C1B-A6E2DCD9979D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$476</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -520,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U476"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T451" sqref="T451"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22888,7 +22893,7 @@
         <v>1590</v>
       </c>
       <c r="U308">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.3">
@@ -24043,7 +24048,7 @@
         <v>1590</v>
       </c>
       <c r="U324">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="325" spans="1:21" x14ac:dyDescent="0.3">
@@ -25211,7 +25216,7 @@
         <v>1590</v>
       </c>
       <c r="U340">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="341" spans="1:21" x14ac:dyDescent="0.3">
@@ -26379,7 +26384,7 @@
         <v>1590</v>
       </c>
       <c r="U356">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="357" spans="1:21" x14ac:dyDescent="0.3">
@@ -27547,7 +27552,7 @@
         <v>1590</v>
       </c>
       <c r="U372">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="373" spans="1:21" x14ac:dyDescent="0.3">
@@ -28712,7 +28717,7 @@
         <v>1590</v>
       </c>
       <c r="U388">
-        <v>17.600000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="389" spans="1:21" x14ac:dyDescent="0.3">
@@ -30962,7 +30967,7 @@
         <v>1805</v>
       </c>
       <c r="U419">
-        <v>17.600000000000001</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="420" spans="1:21" x14ac:dyDescent="0.3">
@@ -32130,7 +32135,7 @@
         <v>1805</v>
       </c>
       <c r="U435">
-        <v>17.600000000000001</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="436" spans="1:21" x14ac:dyDescent="0.3">
@@ -33240,7 +33245,7 @@
         <v>1805</v>
       </c>
       <c r="U451">
-        <v>17.600000000000001</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="452" spans="1:21" x14ac:dyDescent="0.3">
@@ -33893,6 +33898,7 @@
       <c r="L476" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U476" xr:uid="{75299AE7-023E-401C-8CE3-3E0A30A6E256}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>